<commit_message>
corrected a couple errors in biomass equation assignments
</commit_message>
<xml_diff>
--- a/ARB_Volume_and_Biomass_Tables.xlsx
+++ b/ARB_Volume_and_Biomass_Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="269">
   <si>
     <t>bigleaf maple</t>
   </si>
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t>Singleleaf pinyon</t>
-  </si>
-  <si>
-    <t>13</t>
   </si>
   <si>
     <t>Redwood (when DBH &gt; 39.37 inches)</t>
@@ -865,19 +862,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -945,15 +936,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -962,10 +950,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -974,8 +962,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1274,111 +1267,111 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="162.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="162.85546875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="9"/>
+    </row>
+    <row r="28" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" s="6" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-    </row>
-    <row r="28" spans="2:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" s="7" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1407,21 +1400,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1584,16 +1577,16 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>51</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>51</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>51</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>51</v>
       </c>
     </row>
@@ -1640,16 +1633,16 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>56</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>56</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>56</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>56</v>
       </c>
     </row>
@@ -2000,16 +1993,16 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>130</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="4">
         <v>130</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="4">
         <v>130</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="4">
         <v>130</v>
       </c>
     </row>
@@ -2198,28 +2191,28 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="4">
         <v>298</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="4">
         <v>298</v>
       </c>
-      <c r="C61" s="5">
+      <c r="C61" s="4">
         <v>298</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="4">
         <v>298</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+      <c r="A62" s="4">
         <v>299</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="4">
         <v>299</v>
       </c>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -2250,16 +2243,16 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="4">
         <v>320</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="4">
         <v>320</v>
       </c>
-      <c r="C65" s="5">
+      <c r="C65" s="4">
         <v>320</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="4">
         <v>320</v>
       </c>
     </row>
@@ -2278,16 +2271,16 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67" s="4">
         <v>322</v>
       </c>
-      <c r="B67" s="5">
+      <c r="B67" s="4">
         <v>322</v>
       </c>
-      <c r="C67" s="5">
+      <c r="C67" s="4">
         <v>322</v>
       </c>
-      <c r="D67" s="5">
+      <c r="D67" s="4">
         <v>322</v>
       </c>
     </row>
@@ -2474,66 +2467,66 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-      <c r="B81" s="5">
+      <c r="A81" s="4"/>
+      <c r="B81" s="4">
         <v>540</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
+      <c r="A82" s="4">
         <v>542</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="4">
         <v>542</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C82" s="4">
         <v>542</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D82" s="4">
         <v>542</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="5">
+      <c r="A83" s="4">
         <v>547</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="4">
         <v>547</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C83" s="4">
         <v>547</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="4">
         <v>547</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="5">
+      <c r="A84" s="4">
         <v>590</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="4">
         <v>590</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="4">
         <v>590</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D84" s="4">
         <v>590</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="5">
+      <c r="A85" s="4">
         <v>591</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="4">
         <v>591</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C85" s="4">
         <v>591</v>
       </c>
-      <c r="D85" s="5">
+      <c r="D85" s="4">
         <v>591</v>
       </c>
     </row>
@@ -2999,16 +2992,16 @@
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="5">
+      <c r="A120" s="4">
         <v>929</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="4">
         <v>929</v>
       </c>
-      <c r="C120" s="5">
+      <c r="C120" s="4">
         <v>929</v>
       </c>
-      <c r="D120" s="5">
+      <c r="D120" s="4">
         <v>929</v>
       </c>
     </row>
@@ -3113,22 +3106,22 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" t="s">
         <v>237</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>240</v>
       </c>
-      <c r="G1" t="s">
-        <v>241</v>
-      </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4422,22 +4415,22 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D1" t="s">
         <v>237</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>238</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>239</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>240</v>
       </c>
-      <c r="G1" t="s">
-        <v>241</v>
-      </c>
       <c r="H1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5223,29 +5216,29 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>755</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="2">
+      <c r="C36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="1">
         <v>46</v>
       </c>
       <c r="H36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -5881,7 +5874,7 @@
         <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6053,20 +6046,20 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>51</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.41</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>25.58</v>
       </c>
       <c r="E14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6112,20 +6105,20 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.41</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>25.58</v>
       </c>
       <c r="E18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6675,20 +6668,20 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>298</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>0.41</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>25.58</v>
       </c>
       <c r="E58" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -6715,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,7 +6734,7 @@
         <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -6801,20 +6794,20 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>322</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.47</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>29.33</v>
       </c>
       <c r="E6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -7028,37 +7021,37 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>547</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.51</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>31.82</v>
       </c>
       <c r="E22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>590</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.5</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>31.2</v>
       </c>
       <c r="E23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -7230,20 +7223,20 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>755</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>0.78</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>48.67</v>
       </c>
       <c r="E36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -7527,20 +7520,20 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>929</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="D57" s="1">
+        <v>22.46</v>
+      </c>
+      <c r="E57" t="s">
         <v>226</v>
-      </c>
-      <c r="C57" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="D57" s="2">
-        <v>22.46</v>
-      </c>
-      <c r="E57" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -7623,8 +7616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7640,22 +7633,22 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>244</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>245</v>
       </c>
-      <c r="G1" t="s">
-        <v>246</v>
-      </c>
       <c r="H1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7912,29 +7905,29 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>51</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="1">
         <v>13</v>
       </c>
       <c r="H13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -8582,29 +8575,29 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>130</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>14</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" s="2" t="s">
+      <c r="D42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -8727,7 +8720,7 @@
         <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C48">
         <v>17</v>
@@ -8750,10 +8743,10 @@
         <v>211</v>
       </c>
       <c r="B49" t="s">
-        <v>199</v>
-      </c>
-      <c r="C49" t="s">
-        <v>197</v>
+        <v>198</v>
+      </c>
+      <c r="C49">
+        <v>13</v>
       </c>
       <c r="D49">
         <v>13</v>
@@ -8773,7 +8766,7 @@
         <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C50">
         <v>17</v>
@@ -8796,7 +8789,7 @@
         <v>212</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C51">
         <v>13</v>
@@ -8961,8 +8954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8978,22 +8971,22 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" t="s">
         <v>242</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>243</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>244</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>245</v>
       </c>
-      <c r="G1" t="s">
-        <v>246</v>
-      </c>
       <c r="H1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -9089,29 +9082,29 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>322</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -9414,25 +9407,25 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>542</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" s="5">
+      <c r="C20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="4">
         <v>39</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" s="5">
+      <c r="E20" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="4">
         <v>39</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="4" t="s">
         <v>114</v>
       </c>
     </row>
@@ -9483,29 +9476,29 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>591</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>27</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>27</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>27</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>27</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>27</v>
       </c>
       <c r="H23" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -9536,7 +9529,7 @@
         <v>603</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" t="s">
         <v>114</v>
@@ -9559,7 +9552,7 @@
         <v>604</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
         <v>114</v>
@@ -9582,7 +9575,7 @@
         <v>611</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" t="s">
         <v>114</v>
@@ -9628,7 +9621,7 @@
         <v>660</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29">
         <v>37</v>
@@ -9651,7 +9644,7 @@
         <v>661</v>
       </c>
       <c r="B30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C30">
         <v>37</v>
@@ -9785,29 +9778,29 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>755</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -9815,7 +9808,7 @@
         <v>756</v>
       </c>
       <c r="B37" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s">
         <v>114</v>
@@ -9838,7 +9831,7 @@
         <v>758</v>
       </c>
       <c r="B38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C38" t="s">
         <v>114</v>
@@ -9861,7 +9854,7 @@
         <v>760</v>
       </c>
       <c r="B39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C39">
         <v>27</v>
@@ -10160,7 +10153,7 @@
         <v>850</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C52" t="s">
         <v>114</v>
@@ -10438,10 +10431,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10456,23 +10449,23 @@
       <c r="B1" t="s">
         <v>109</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="G1" t="s">
-        <v>236</v>
-      </c>
       <c r="H1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -10482,19 +10475,19 @@
       <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="12">
         <v>18</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="12">
         <v>18</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="12">
         <v>18</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="12">
         <v>18</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="12">
         <v>18</v>
       </c>
     </row>
@@ -10505,19 +10498,19 @@
       <c r="B3" t="s">
         <v>113</v>
       </c>
-      <c r="C3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3">
+      <c r="C3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="12">
         <v>1</v>
       </c>
     </row>
@@ -10528,19 +10521,19 @@
       <c r="B4" t="s">
         <v>115</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="12">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="12">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="12">
         <v>1</v>
       </c>
     </row>
@@ -10551,19 +10544,19 @@
       <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="12">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>1</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="12">
         <v>1</v>
       </c>
     </row>
@@ -10574,19 +10567,19 @@
       <c r="B6" t="s">
         <v>117</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="12">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>2</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="12">
         <v>2</v>
       </c>
     </row>
@@ -10597,19 +10590,19 @@
       <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="12">
         <v>2</v>
       </c>
-      <c r="F7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" s="12">
         <v>3</v>
       </c>
     </row>
@@ -10620,19 +10613,19 @@
       <c r="B8" t="s">
         <v>61</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <v>3</v>
       </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="12">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="12">
         <v>3</v>
       </c>
     </row>
@@ -10643,19 +10636,19 @@
       <c r="B9" t="s">
         <v>118</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="12">
         <v>3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="12">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <v>3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="12">
         <v>3</v>
       </c>
     </row>
@@ -10666,19 +10659,19 @@
       <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <v>10</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
         <v>10</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="12">
         <v>10</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <v>10</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10689,19 +10682,19 @@
       <c r="B11" t="s">
         <v>147</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="12">
         <v>19</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="12">
         <v>19</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="12">
         <v>19</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <v>19</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10712,46 +10705,46 @@
       <c r="B12" t="s">
         <v>119</v>
       </c>
-      <c r="C12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12">
+      <c r="C12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G12" s="12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>51</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="C13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="13">
         <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -10761,19 +10754,19 @@
       <c r="B14" t="s">
         <v>121</v>
       </c>
-      <c r="C14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" t="s">
-        <v>114</v>
-      </c>
-      <c r="F14" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14">
+      <c r="C14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10784,19 +10777,19 @@
       <c r="B15" t="s">
         <v>67</v>
       </c>
-      <c r="C15" t="s">
-        <v>114</v>
-      </c>
-      <c r="D15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" t="s">
-        <v>114</v>
-      </c>
-      <c r="F15" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15">
+      <c r="C15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10807,19 +10800,19 @@
       <c r="B16" t="s">
         <v>122</v>
       </c>
-      <c r="C16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D16" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F16" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16">
+      <c r="C16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10830,19 +10823,19 @@
       <c r="B17" t="s">
         <v>194</v>
       </c>
-      <c r="C17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" t="s">
-        <v>114</v>
-      </c>
-      <c r="E17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17">
+      <c r="C17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="12">
         <v>10</v>
       </c>
     </row>
@@ -10853,19 +10846,19 @@
       <c r="B18" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" t="s">
-        <v>114</v>
-      </c>
-      <c r="F18" t="s">
-        <v>114</v>
-      </c>
-      <c r="G18">
+      <c r="C18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="12">
         <v>13</v>
       </c>
     </row>
@@ -10876,19 +10869,19 @@
       <c r="B19" t="s">
         <v>124</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="12">
         <v>13</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="12">
         <v>13</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="12">
         <v>13</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="12">
         <v>13</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="12">
         <v>13</v>
       </c>
     </row>
@@ -10899,19 +10892,19 @@
       <c r="B20" t="s">
         <v>71</v>
       </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>114</v>
-      </c>
-      <c r="E20" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20">
+      <c r="C20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" s="12">
         <v>13</v>
       </c>
     </row>
@@ -10922,19 +10915,19 @@
       <c r="B21" t="s">
         <v>125</v>
       </c>
-      <c r="C21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21">
+      <c r="C21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="12">
         <v>13</v>
       </c>
-      <c r="F21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21">
+      <c r="F21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="12">
         <v>13</v>
       </c>
     </row>
@@ -10945,19 +10938,19 @@
       <c r="B22" t="s">
         <v>195</v>
       </c>
-      <c r="C22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="12">
         <v>20</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="12">
         <v>20</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="12">
         <v>20</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" s="12" t="s">
         <v>114</v>
       </c>
     </row>
@@ -10968,19 +10961,19 @@
       <c r="B23" t="s">
         <v>127</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12">
         <v>20</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="12">
         <v>20</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="12">
         <v>20</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="12">
         <v>20</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="12">
         <v>20</v>
       </c>
     </row>
@@ -10991,19 +10984,19 @@
       <c r="B24" t="s">
         <v>128</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12">
         <v>10</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="12">
         <v>10</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="12">
         <v>10</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="12">
         <v>10</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="12">
         <v>10</v>
       </c>
     </row>
@@ -11014,19 +11007,19 @@
       <c r="B25" t="s">
         <v>77</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="12">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25">
+      <c r="D25" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="12">
         <v>4</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="12">
         <v>4</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="12">
         <v>4</v>
       </c>
     </row>
@@ -11037,19 +11030,19 @@
       <c r="B26" t="s">
         <v>78</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="12">
         <v>4</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="12">
         <v>4</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="12">
         <v>4</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="12">
         <v>4</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="12">
         <v>4</v>
       </c>
     </row>
@@ -11060,19 +11053,19 @@
       <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="12">
         <v>5</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="12">
         <v>5</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="12">
         <v>5</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="12">
         <v>5</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="12">
         <v>5</v>
       </c>
     </row>
@@ -11083,19 +11076,19 @@
       <c r="B28" t="s">
         <v>129</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="12">
         <v>9</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="12">
         <v>9</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="12">
         <v>9</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="12">
         <v>9</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11106,19 +11099,19 @@
       <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G29">
+      <c r="C29" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11129,19 +11122,19 @@
       <c r="B30" t="s">
         <v>130</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="12">
         <v>11</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="12">
         <v>11</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="12">
         <v>11</v>
       </c>
-      <c r="F30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G30">
+      <c r="F30" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11152,19 +11145,19 @@
       <c r="B31" t="s">
         <v>131</v>
       </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" t="s">
-        <v>114</v>
-      </c>
-      <c r="G31">
+      <c r="C31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11175,19 +11168,19 @@
       <c r="B32" t="s">
         <v>132</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="12">
         <v>11</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="12">
         <v>11</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="12">
         <v>11</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="12">
         <v>11</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11198,19 +11191,19 @@
       <c r="B33" t="s">
         <v>86</v>
       </c>
-      <c r="C33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" t="s">
-        <v>114</v>
-      </c>
-      <c r="E33" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33">
+      <c r="C33" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" s="12">
         <v>7</v>
       </c>
     </row>
@@ -11221,19 +11214,19 @@
       <c r="B34" t="s">
         <v>133</v>
       </c>
-      <c r="C34" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34">
+      <c r="C34" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="12">
         <v>11</v>
       </c>
-      <c r="F34" t="s">
-        <v>114</v>
-      </c>
-      <c r="G34">
+      <c r="F34" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11244,19 +11237,19 @@
       <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="12">
         <v>7</v>
       </c>
-      <c r="D35" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35">
+      <c r="D35" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="12">
         <v>7</v>
       </c>
-      <c r="F35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G35">
+      <c r="F35" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" s="12">
         <v>7</v>
       </c>
     </row>
@@ -11267,19 +11260,19 @@
       <c r="B36" t="s">
         <v>134</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="12">
         <v>8</v>
       </c>
-      <c r="D36" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36">
+      <c r="D36" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E36" s="12">
         <v>8</v>
       </c>
-      <c r="F36" t="s">
-        <v>114</v>
-      </c>
-      <c r="G36">
+      <c r="F36" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" s="12">
         <v>8</v>
       </c>
     </row>
@@ -11290,19 +11283,19 @@
       <c r="B37" t="s">
         <v>135</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="12">
         <v>9</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="12">
         <v>9</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="12">
         <v>9</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="12">
         <v>9</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="12">
         <v>9</v>
       </c>
     </row>
@@ -11313,19 +11306,19 @@
       <c r="B38" t="s">
         <v>136</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="12">
         <v>11</v>
       </c>
-      <c r="D38" t="s">
-        <v>114</v>
-      </c>
-      <c r="E38">
+      <c r="D38" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E38" s="12">
         <v>11</v>
       </c>
-      <c r="F38" t="s">
-        <v>114</v>
-      </c>
-      <c r="G38">
+      <c r="F38" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11336,19 +11329,19 @@
       <c r="B39" t="s">
         <v>137</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="12">
         <v>7</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="12">
         <v>7</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="12">
         <v>7</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="12">
         <v>7</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="12">
         <v>7</v>
       </c>
     </row>
@@ -11359,19 +11352,19 @@
       <c r="B40" t="s">
         <v>93</v>
       </c>
-      <c r="C40" t="s">
-        <v>114</v>
-      </c>
-      <c r="D40" t="s">
-        <v>114</v>
-      </c>
-      <c r="E40" t="s">
-        <v>114</v>
-      </c>
-      <c r="F40" t="s">
-        <v>114</v>
-      </c>
-      <c r="G40">
+      <c r="C40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11382,19 +11375,19 @@
       <c r="B41" t="s">
         <v>138</v>
       </c>
-      <c r="C41" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41" t="s">
-        <v>114</v>
-      </c>
-      <c r="F41" t="s">
-        <v>114</v>
-      </c>
-      <c r="G41">
+      <c r="C41" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="12">
         <v>7</v>
       </c>
     </row>
@@ -11405,19 +11398,19 @@
       <c r="B42" t="s">
         <v>95</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="12">
         <v>11</v>
       </c>
-      <c r="D42" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" t="s">
-        <v>114</v>
-      </c>
-      <c r="G42" t="s">
+      <c r="D42" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>114</v>
       </c>
     </row>
@@ -11428,19 +11421,19 @@
       <c r="B43" t="s">
         <v>196</v>
       </c>
-      <c r="C43" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" t="s">
-        <v>114</v>
-      </c>
-      <c r="E43" t="s">
-        <v>114</v>
-      </c>
-      <c r="F43" t="s">
-        <v>114</v>
-      </c>
-      <c r="G43">
+      <c r="C43" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" s="12">
         <v>11</v>
       </c>
     </row>
@@ -11451,19 +11444,19 @@
       <c r="B44" t="s">
         <v>97</v>
       </c>
-      <c r="C44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" t="s">
-        <v>114</v>
-      </c>
-      <c r="G44">
+      <c r="C44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G44" s="12">
         <v>7</v>
       </c>
     </row>
@@ -11474,66 +11467,66 @@
       <c r="B45" t="s">
         <v>98</v>
       </c>
-      <c r="C45" t="s">
-        <v>114</v>
-      </c>
-      <c r="D45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E45" t="s">
-        <v>114</v>
-      </c>
-      <c r="F45" t="s">
-        <v>114</v>
-      </c>
-      <c r="G45">
+      <c r="C45" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G45" s="12">
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>201</v>
       </c>
       <c r="B46" t="s">
         <v>148</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G46" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C46" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" s="14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>202</v>
       </c>
       <c r="B47" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="1">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1">
-        <v>8</v>
-      </c>
-      <c r="E47" s="1">
-        <v>25</v>
-      </c>
-      <c r="F47" s="1">
-        <v>25</v>
-      </c>
-      <c r="G47" s="1">
-        <v>8</v>
+      <c r="C47" s="14">
+        <v>6</v>
+      </c>
+      <c r="D47" s="14">
+        <v>6</v>
+      </c>
+      <c r="E47" s="14">
+        <v>22</v>
+      </c>
+      <c r="F47" s="14">
+        <v>22</v>
+      </c>
+      <c r="G47" s="14">
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -11541,233 +11534,188 @@
         <v>211</v>
       </c>
       <c r="B48" t="s">
-        <v>198</v>
-      </c>
-      <c r="C48">
-        <v>17</v>
-      </c>
-      <c r="D48">
-        <v>17</v>
-      </c>
-      <c r="E48">
-        <v>17</v>
-      </c>
-      <c r="F48">
-        <v>17</v>
-      </c>
-      <c r="G48">
-        <v>17</v>
+        <v>140</v>
+      </c>
+      <c r="C48" s="12">
+        <v>10</v>
+      </c>
+      <c r="D48" s="12">
+        <v>10</v>
+      </c>
+      <c r="E48" s="12">
+        <v>10</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B49" t="s">
-        <v>199</v>
-      </c>
-      <c r="C49" t="s">
-        <v>197</v>
-      </c>
-      <c r="D49">
-        <v>13</v>
-      </c>
-      <c r="E49">
-        <v>13</v>
-      </c>
-      <c r="F49">
-        <v>13</v>
-      </c>
-      <c r="G49">
-        <v>13</v>
+        <v>141</v>
+      </c>
+      <c r="C49" s="12">
+        <v>10</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E49" s="12">
+        <v>10</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G49" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="B50" t="s">
-        <v>200</v>
-      </c>
-      <c r="C50">
-        <v>17</v>
-      </c>
-      <c r="D50" t="s">
-        <v>114</v>
-      </c>
-      <c r="E50">
-        <v>17</v>
-      </c>
-      <c r="F50" t="s">
-        <v>114</v>
-      </c>
-      <c r="G50">
-        <v>17</v>
+        <v>103</v>
+      </c>
+      <c r="C50" s="12">
+        <v>10</v>
+      </c>
+      <c r="D50" s="12">
+        <v>10</v>
+      </c>
+      <c r="E50" s="12">
+        <v>10</v>
+      </c>
+      <c r="F50" s="12">
+        <v>10</v>
+      </c>
+      <c r="G50" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>212</v>
+        <v>242</v>
       </c>
       <c r="B51" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>114</v>
-      </c>
-      <c r="E51">
-        <v>13</v>
-      </c>
-      <c r="F51" t="s">
-        <v>114</v>
-      </c>
-      <c r="G51">
-        <v>13</v>
+        <v>142</v>
+      </c>
+      <c r="C51" s="12">
+        <v>10</v>
+      </c>
+      <c r="D51" s="12">
+        <v>10</v>
+      </c>
+      <c r="E51" s="12">
+        <v>10</v>
+      </c>
+      <c r="F51" s="12">
+        <v>10</v>
+      </c>
+      <c r="G51" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52">
-        <v>38</v>
-      </c>
-      <c r="D52">
-        <v>13</v>
-      </c>
-      <c r="E52">
-        <v>13</v>
-      </c>
-      <c r="F52">
-        <v>38</v>
-      </c>
-      <c r="G52">
-        <v>13</v>
+        <v>143</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" s="12">
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>242</v>
+        <v>263</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53">
-        <v>38</v>
-      </c>
-      <c r="D53">
-        <v>13</v>
-      </c>
-      <c r="E53">
-        <v>13</v>
-      </c>
-      <c r="F53">
-        <v>13</v>
-      </c>
-      <c r="G53">
-        <v>13</v>
+        <v>144</v>
+      </c>
+      <c r="C53" s="12">
+        <v>23</v>
+      </c>
+      <c r="D53" s="12">
+        <v>23</v>
+      </c>
+      <c r="E53" s="12">
+        <v>23</v>
+      </c>
+      <c r="F53" s="12">
+        <v>23</v>
+      </c>
+      <c r="G53" s="12">
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
-      </c>
-      <c r="C54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" t="s">
-        <v>114</v>
-      </c>
-      <c r="E54" t="s">
-        <v>114</v>
-      </c>
-      <c r="F54" t="s">
-        <v>114</v>
-      </c>
-      <c r="G54">
-        <v>13</v>
+        <v>145</v>
+      </c>
+      <c r="C54" s="12">
+        <v>24</v>
+      </c>
+      <c r="D54" s="12">
+        <v>24</v>
+      </c>
+      <c r="E54" s="12">
+        <v>24</v>
+      </c>
+      <c r="F54" s="12">
+        <v>24</v>
+      </c>
+      <c r="G54" s="12">
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>263</v>
+        <v>298</v>
       </c>
       <c r="B55" t="s">
-        <v>144</v>
-      </c>
-      <c r="C55">
-        <v>26</v>
-      </c>
-      <c r="D55">
-        <v>26</v>
-      </c>
-      <c r="E55">
-        <v>26</v>
-      </c>
-      <c r="F55">
-        <v>26</v>
-      </c>
-      <c r="G55">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>264</v>
-      </c>
-      <c r="B56" t="s">
-        <v>145</v>
-      </c>
-      <c r="C56">
-        <v>21</v>
-      </c>
-      <c r="D56">
-        <v>21</v>
-      </c>
-      <c r="E56">
-        <v>21</v>
-      </c>
-      <c r="F56">
-        <v>21</v>
-      </c>
-      <c r="G56">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>298</v>
-      </c>
-      <c r="B57" t="s">
         <v>146</v>
       </c>
-      <c r="C57">
-        <v>21</v>
-      </c>
-      <c r="D57">
-        <v>21</v>
-      </c>
-      <c r="E57">
-        <v>21</v>
-      </c>
-      <c r="F57">
-        <v>21</v>
-      </c>
-      <c r="G57">
-        <v>21</v>
+      <c r="C55" s="12">
+        <v>24</v>
+      </c>
+      <c r="D55" s="12">
+        <v>24</v>
+      </c>
+      <c r="E55" s="12">
+        <v>24</v>
+      </c>
+      <c r="F55" s="12">
+        <v>24</v>
+      </c>
+      <c r="G55" s="12">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11775,8 +11723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11792,22 +11740,22 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
         <v>232</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>233</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>234</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>235</v>
       </c>
-      <c r="G1" t="s">
-        <v>236</v>
-      </c>
       <c r="H1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -11857,29 +11805,29 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>320</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -11906,29 +11854,29 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>322</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -12208,29 +12156,29 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>511</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G19" s="2">
+      <c r="C19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G19" s="1">
         <v>28</v>
       </c>
       <c r="H19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -12257,29 +12205,29 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>547</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" s="2" t="s">
+      <c r="C21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>114</v>
       </c>
       <c r="H21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -12356,7 +12304,7 @@
         <v>603</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C25" t="s">
         <v>114</v>
@@ -12379,7 +12327,7 @@
         <v>604</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C26" t="s">
         <v>114</v>
@@ -12402,7 +12350,7 @@
         <v>611</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" t="s">
         <v>114</v>
@@ -12586,7 +12534,7 @@
         <v>755</v>
       </c>
       <c r="B35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C35" t="s">
         <v>114</v>
@@ -12609,7 +12557,7 @@
         <v>756</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C36" t="s">
         <v>114</v>
@@ -12632,7 +12580,7 @@
         <v>758</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C37" t="s">
         <v>114</v>

</xml_diff>